<commit_message>
Deng, Hooi 2021 - 2nd Readthrough
</commit_message>
<xml_diff>
--- a/3_Categorisation/Categorie-Methode liste.xlsx
+++ b/3_Categorisation/Categorie-Methode liste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Documents\Cours\KIT\11_HK\AD\3_Categorisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25A1BB5-F21B-4B86-B685-887DC7A7D7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108B9DDD-FB30-4E48-98B5-AC3D0E39BE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{AE90E999-193C-4C0E-9858-77EC5F42F2A6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="309">
   <si>
     <t>Parent</t>
   </si>
@@ -1602,11 +1602,11 @@
   <dimension ref="F3:W999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="11" ySplit="7" topLeftCell="N110" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="7" topLeftCell="N31" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
-      <selection pane="bottomRight" activeCell="I136" sqref="I136"/>
+      <selection pane="bottomRight" activeCell="N89" sqref="N89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -4110,13 +4110,19 @@
         <f>IF(Table1[[#This Row],[Children]]=0,"",Table1[[#This Row],[Children]])</f>
         <v/>
       </c>
-      <c r="N70" s="13"/>
+      <c r="N70" s="13">
+        <v>0.8</v>
+      </c>
       <c r="O70" s="5"/>
       <c r="P70" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="Q70" s="5"/>
-      <c r="R70" s="5"/>
+      <c r="Q70" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="R70" s="5" t="s">
+        <v>193</v>
+      </c>
       <c r="S70" s="13"/>
       <c r="T70" s="6" t="s">
         <v>307</v>

</xml_diff>